<commit_message>
- Documentation file corected
</commit_message>
<xml_diff>
--- a/SimpleChatApp_Documentation.xlsx
+++ b/SimpleChatApp_Documentation.xlsx
@@ -233,7 +233,7 @@
     <t>1.0.3.</t>
   </si>
   <si>
-    <t>16/11/2017</t>
+    <t>30/11/2017</t>
   </si>
 </sst>
 </file>
@@ -692,6 +692,20 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -699,20 +713,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,7 +1055,7 @@
   <dimension ref="B3:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1070,56 +1070,56 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="2:6" ht="19.899999999999999" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="8" spans="2:6">
       <c r="B8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6">
@@ -1136,11 +1136,11 @@
       <c r="B12" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1">
       <c r="B13" s="27" t="s">
@@ -1167,21 +1167,21 @@
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="35">
         <v>42959</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="38" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -1190,19 +1190,19 @@
       <c r="D19" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>